<commit_message>
En cours : Completer animation
</commit_message>
<xml_diff>
--- a/BackLogAndSprint2Android.xlsx
+++ b/BackLogAndSprint2Android.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre\Desktop\Projet-Android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E71D47-B1A9-4B63-B0C6-6F1CFFAD630E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9645ED0A-4B3A-40D2-A15C-B64FA6B30F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{73B89499-F026-470B-8F3E-C42C4C713BCD}"/>
+    <workbookView minimized="1" xWindow="-25200" yWindow="2040" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{73B89499-F026-470B-8F3E-C42C4C713BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +151,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -165,12 +171,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -488,7 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5F4C72-E276-4517-9B7C-25770706BFAF}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -681,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C985D0-9DA0-44F0-9CF9-DDB0C920DF2C}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +715,7 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -716,7 +723,7 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -724,7 +731,7 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -732,7 +739,7 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reste a stretch l'image et l'animation
</commit_message>
<xml_diff>
--- a/BackLogAndSprint2Android.xlsx
+++ b/BackLogAndSprint2Android.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre\Desktop\Projet-Android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9645ED0A-4B3A-40D2-A15C-B64FA6B30F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B3A754-FE0D-4F2B-B553-693690C529E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-25200" yWindow="2040" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{73B89499-F026-470B-8F3E-C42C4C713BCD}"/>
+    <workbookView xWindow="-25320" yWindow="390" windowWidth="25440" windowHeight="15990" activeTab="1" xr2:uid="{73B89499-F026-470B-8F3E-C42C4C713BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -689,7 +689,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +769,7 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -777,7 +777,7 @@
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -791,7 +791,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>